<commit_message>
SaveAs data file formats in .xlsx
</commit_message>
<xml_diff>
--- a/NRI_STLF_Data/WeatherData/T_hamedan/T_hamedan91.xlsx
+++ b/NRI_STLF_Data/WeatherData/T_hamedan/T_hamedan91.xlsx
@@ -46,11 +46,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -381,13 +381,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="G133" sqref="G133"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27">
       <c r="A1">
         <v>91</v>
       </c>
@@ -452,7 +452,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27">
       <c r="A2">
         <v>91</v>
       </c>
@@ -529,7 +529,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27">
       <c r="A3">
         <v>91</v>
       </c>
@@ -609,7 +609,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27">
       <c r="A4">
         <v>91</v>
       </c>
@@ -686,7 +686,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27">
       <c r="A5">
         <v>91</v>
       </c>
@@ -763,7 +763,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27">
       <c r="A6">
         <v>91</v>
       </c>
@@ -828,7 +828,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27">
       <c r="A7">
         <v>91</v>
       </c>
@@ -893,7 +893,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27">
       <c r="A8">
         <v>91</v>
       </c>
@@ -976,7 +976,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27">
       <c r="A9">
         <v>91</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27">
       <c r="A10">
         <v>91</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27">
       <c r="A11">
         <v>91</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27">
       <c r="A12">
         <v>91</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27">
       <c r="A13">
         <v>91</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27">
       <c r="A14">
         <v>91</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27">
       <c r="A15">
         <v>91</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27">
       <c r="A16">
         <v>91</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27">
       <c r="A17">
         <v>91</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27">
       <c r="A18">
         <v>91</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27">
       <c r="A19">
         <v>91</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27">
       <c r="A20">
         <v>91</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27">
       <c r="A21">
         <v>91</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27">
       <c r="A22">
         <v>91</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27">
       <c r="A23">
         <v>91</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27">
       <c r="A24">
         <v>91</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27">
       <c r="A25">
         <v>91</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27">
       <c r="A26">
         <v>91</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27">
       <c r="A27">
         <v>91</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27">
       <c r="A28">
         <v>91</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27">
       <c r="A29">
         <v>91</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27">
       <c r="A30">
         <v>91</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27">
       <c r="A31">
         <v>91</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27">
       <c r="A32">
         <v>91</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27">
       <c r="A33">
         <v>91</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27">
       <c r="A34">
         <v>91</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27">
       <c r="A35">
         <v>91</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27">
       <c r="A36">
         <v>91</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27">
       <c r="A37">
         <v>91</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27">
       <c r="A38">
         <v>91</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27">
       <c r="A39">
         <v>91</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27">
       <c r="A40">
         <v>91</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27">
       <c r="A41">
         <v>91</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27">
       <c r="A42">
         <v>91</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27">
       <c r="A43">
         <v>91</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27">
       <c r="A44">
         <v>91</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27">
       <c r="A45">
         <v>91</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27">
       <c r="A46">
         <v>91</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27">
       <c r="A47">
         <v>91</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27">
       <c r="A48">
         <v>91</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27">
       <c r="A49">
         <v>91</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27">
       <c r="A50">
         <v>91</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27">
       <c r="A51">
         <v>91</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27">
       <c r="A52">
         <v>91</v>
       </c>
@@ -4436,7 +4436,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27">
       <c r="A53">
         <v>91</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:27">
       <c r="A54">
         <v>91</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:27">
       <c r="A55">
         <v>91</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:27">
       <c r="A56">
         <v>91</v>
       </c>
@@ -4744,7 +4744,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:27">
       <c r="A57">
         <v>91</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:27">
       <c r="A58">
         <v>91</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:27">
       <c r="A59">
         <v>91</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27">
       <c r="A60">
         <v>91</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:27">
       <c r="A61">
         <v>91</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:27">
       <c r="A62">
         <v>91</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:27">
       <c r="A63">
         <v>91</v>
       </c>
@@ -5286,7 +5286,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:27">
       <c r="A64">
         <v>91</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:27">
       <c r="A65">
         <v>91</v>
       </c>
@@ -5449,7 +5449,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:27">
       <c r="A66">
         <v>91</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:27">
       <c r="A67">
         <v>91</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:27">
       <c r="A68">
         <v>91</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:27">
       <c r="A69">
         <v>91</v>
       </c>
@@ -5763,7 +5763,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:27">
       <c r="A70">
         <v>91</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:27">
       <c r="A71">
         <v>91</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:27">
       <c r="A72">
         <v>91</v>
       </c>
@@ -5991,7 +5991,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:27">
       <c r="A73">
         <v>91</v>
       </c>
@@ -6068,7 +6068,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:27">
       <c r="A74">
         <v>91</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:27">
       <c r="A75">
         <v>91</v>
       </c>
@@ -6210,7 +6210,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:27">
       <c r="A76">
         <v>91</v>
       </c>
@@ -6275,7 +6275,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:27">
       <c r="A77">
         <v>91</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:27">
       <c r="A78">
         <v>91</v>
       </c>
@@ -6429,7 +6429,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:27">
       <c r="A79">
         <v>91</v>
       </c>
@@ -6506,7 +6506,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:27">
       <c r="A80">
         <v>91</v>
       </c>
@@ -6583,7 +6583,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:27">
       <c r="A81">
         <v>91</v>
       </c>
@@ -6660,7 +6660,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:27">
       <c r="A82">
         <v>91</v>
       </c>
@@ -6725,7 +6725,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:27">
       <c r="A83">
         <v>91</v>
       </c>
@@ -6802,7 +6802,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:27">
       <c r="A84">
         <v>91</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:27">
       <c r="A85">
         <v>91</v>
       </c>
@@ -6962,7 +6962,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:27">
       <c r="A86">
         <v>91</v>
       </c>
@@ -7039,7 +7039,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:27">
       <c r="A87">
         <v>91</v>
       </c>
@@ -7119,7 +7119,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:27">
       <c r="A88">
         <v>91</v>
       </c>
@@ -7196,7 +7196,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:27">
       <c r="A89">
         <v>91</v>
       </c>
@@ -7273,7 +7273,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:27">
       <c r="A90">
         <v>91</v>
       </c>
@@ -7350,7 +7350,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:27">
       <c r="A91">
         <v>91</v>
       </c>
@@ -7427,7 +7427,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:27">
       <c r="A92">
         <v>91</v>
       </c>
@@ -7504,7 +7504,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:27">
       <c r="A93">
         <v>91</v>
       </c>
@@ -7581,7 +7581,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:27">
       <c r="A94">
         <v>91</v>
       </c>
@@ -7658,7 +7658,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:27">
       <c r="A95">
         <v>91</v>
       </c>
@@ -7735,7 +7735,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:27">
       <c r="A96">
         <v>91</v>
       </c>
@@ -7812,7 +7812,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:27">
       <c r="A97">
         <v>91</v>
       </c>
@@ -7889,7 +7889,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:27">
       <c r="A98">
         <v>91</v>
       </c>
@@ -7966,7 +7966,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:27">
       <c r="A99">
         <v>91</v>
       </c>
@@ -8043,7 +8043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:27">
       <c r="A100">
         <v>91</v>
       </c>
@@ -8120,7 +8120,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:27">
       <c r="A101">
         <v>91</v>
       </c>
@@ -8197,7 +8197,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:27">
       <c r="A102">
         <v>91</v>
       </c>
@@ -8274,7 +8274,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:27">
       <c r="A103">
         <v>91</v>
       </c>
@@ -8351,7 +8351,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:27">
       <c r="A104">
         <v>91</v>
       </c>
@@ -8428,7 +8428,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:27">
       <c r="A105">
         <v>91</v>
       </c>
@@ -8505,7 +8505,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:27">
       <c r="A106">
         <v>91</v>
       </c>
@@ -8570,7 +8570,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:27">
       <c r="A107">
         <v>91</v>
       </c>
@@ -8586,15 +8586,6 @@
       <c r="E107">
         <v>1</v>
       </c>
-      <c r="F107">
-        <v>34</v>
-      </c>
-      <c r="G107">
-        <v>22</v>
-      </c>
-      <c r="H107">
-        <v>11</v>
-      </c>
       <c r="X107">
         <v>0</v>
       </c>
@@ -8602,7 +8593,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:27">
       <c r="A108">
         <v>91</v>
       </c>
@@ -8667,7 +8658,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:27">
       <c r="A109">
         <v>91</v>
       </c>
@@ -8732,7 +8723,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:27">
       <c r="A110">
         <v>91</v>
       </c>
@@ -8797,7 +8788,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:27">
       <c r="A111">
         <v>91</v>
       </c>
@@ -8862,7 +8853,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:27">
       <c r="A112">
         <v>91</v>
       </c>
@@ -8939,7 +8930,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:27">
       <c r="A113">
         <v>91</v>
       </c>
@@ -9016,7 +9007,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:27">
       <c r="A114">
         <v>91</v>
       </c>
@@ -9093,7 +9084,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:27">
       <c r="A115">
         <v>91</v>
       </c>
@@ -9170,7 +9161,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="116" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:27">
       <c r="A116">
         <v>91</v>
       </c>
@@ -9247,7 +9238,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="117" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:27">
       <c r="A117">
         <v>91</v>
       </c>
@@ -9324,7 +9315,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="118" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:27">
       <c r="A118">
         <v>91</v>
       </c>
@@ -9401,7 +9392,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:27">
       <c r="A119">
         <v>91</v>
       </c>
@@ -9481,7 +9472,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="120" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:27">
       <c r="A120">
         <v>91</v>
       </c>
@@ -9558,7 +9549,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="121" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:27">
       <c r="A121">
         <v>91</v>
       </c>
@@ -9635,7 +9626,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="122" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:27">
       <c r="A122">
         <v>91</v>
       </c>
@@ -9712,7 +9703,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="123" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:27">
       <c r="A123">
         <v>91</v>
       </c>
@@ -9795,7 +9786,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="124" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:27">
       <c r="A124">
         <v>91</v>
       </c>
@@ -9878,7 +9869,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="125" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:27">
       <c r="A125">
         <v>91</v>
       </c>
@@ -9958,7 +9949,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="126" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:27">
       <c r="A126">
         <v>91</v>
       </c>
@@ -10038,7 +10029,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="127" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:27">
       <c r="A127">
         <v>91</v>
       </c>
@@ -10115,7 +10106,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="128" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:27">
       <c r="A128">
         <v>91</v>
       </c>
@@ -10192,7 +10183,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="129" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:27">
       <c r="A129">
         <v>91</v>
       </c>
@@ -10269,7 +10260,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="130" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:27">
       <c r="A130">
         <v>91</v>
       </c>
@@ -10346,7 +10337,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="131" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:27">
       <c r="A131">
         <v>91</v>
       </c>
@@ -10426,7 +10417,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="132" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:27">
       <c r="A132">
         <v>91</v>
       </c>
@@ -10503,7 +10494,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="133" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:27">
       <c r="A133">
         <v>91</v>
       </c>
@@ -10522,9 +10513,6 @@
       <c r="F133">
         <v>23</v>
       </c>
-      <c r="G133">
-        <v>26</v>
-      </c>
       <c r="H133">
         <v>23</v>
       </c>
@@ -10580,7 +10568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:27">
       <c r="A134">
         <v>91</v>
       </c>
@@ -10657,7 +10645,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="135" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:27">
       <c r="A135">
         <v>91</v>
       </c>
@@ -10734,7 +10722,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="136" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:27">
       <c r="A136">
         <v>91</v>
       </c>
@@ -10811,7 +10799,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="137" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:27">
       <c r="A137">
         <v>91</v>
       </c>
@@ -10876,7 +10864,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="138" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:27">
       <c r="A138">
         <v>91</v>
       </c>
@@ -10944,7 +10932,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="139" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:27">
       <c r="A139">
         <v>91</v>
       </c>
@@ -11021,7 +11009,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="140" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:27">
       <c r="A140">
         <v>91</v>
       </c>
@@ -11086,7 +11074,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="141" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:27">
       <c r="A141">
         <v>91</v>
       </c>
@@ -11102,15 +11090,6 @@
       <c r="E141">
         <v>1</v>
       </c>
-      <c r="F141">
-        <v>35</v>
-      </c>
-      <c r="G141">
-        <v>25</v>
-      </c>
-      <c r="H141">
-        <v>15</v>
-      </c>
       <c r="X141">
         <v>0</v>
       </c>
@@ -11118,7 +11097,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="142" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:27">
       <c r="A142">
         <v>91</v>
       </c>
@@ -11195,7 +11174,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="143" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:27">
       <c r="A143">
         <v>91</v>
       </c>
@@ -11260,7 +11239,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="144" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:27">
       <c r="A144">
         <v>91</v>
       </c>
@@ -11337,7 +11316,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="145" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:27">
       <c r="A145">
         <v>91</v>
       </c>
@@ -11417,7 +11396,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="146" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:27">
       <c r="A146">
         <v>91</v>
       </c>
@@ -11482,7 +11461,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="147" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:27">
       <c r="A147">
         <v>91</v>
       </c>
@@ -11559,7 +11538,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="148" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:27">
       <c r="A148">
         <v>91</v>
       </c>
@@ -11636,7 +11615,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="149" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:27">
       <c r="A149">
         <v>91</v>
       </c>
@@ -11713,7 +11692,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="150" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:27">
       <c r="A150">
         <v>91</v>
       </c>
@@ -11790,7 +11769,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="151" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:27">
       <c r="A151">
         <v>91</v>
       </c>
@@ -11867,7 +11846,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="152" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:27">
       <c r="A152">
         <v>91</v>
       </c>
@@ -11944,7 +11923,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="153" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:27">
       <c r="A153">
         <v>91</v>
       </c>
@@ -12021,7 +12000,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="154" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:27">
       <c r="A154">
         <v>91</v>
       </c>
@@ -12098,7 +12077,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="155" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:27">
       <c r="A155">
         <v>91</v>
       </c>
@@ -12163,7 +12142,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="156" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:27">
       <c r="A156">
         <v>91</v>
       </c>
@@ -12240,7 +12219,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="157" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:27">
       <c r="A157">
         <v>91</v>
       </c>
@@ -12305,7 +12284,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="158" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:27">
       <c r="A158">
         <v>91</v>
       </c>
@@ -12385,7 +12364,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="159" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:27">
       <c r="A159">
         <v>91</v>
       </c>
@@ -12465,7 +12444,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="160" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:27">
       <c r="A160">
         <v>91</v>
       </c>
@@ -12542,7 +12521,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="161" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:27">
       <c r="A161">
         <v>91</v>
       </c>
@@ -12619,7 +12598,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="162" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:27">
       <c r="A162">
         <v>91</v>
       </c>
@@ -12696,7 +12675,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="163" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:27">
       <c r="A163">
         <v>91</v>
       </c>
@@ -12773,7 +12752,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:27">
       <c r="A164">
         <v>91</v>
       </c>
@@ -12850,7 +12829,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="165" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:27">
       <c r="A165">
         <v>91</v>
       </c>
@@ -12927,7 +12906,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="166" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:27">
       <c r="A166">
         <v>91</v>
       </c>
@@ -13004,7 +12983,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="167" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:27">
       <c r="A167">
         <v>91</v>
       </c>
@@ -13084,7 +13063,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="168" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:27">
       <c r="A168">
         <v>91</v>
       </c>
@@ -13164,7 +13143,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="169" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:27">
       <c r="A169">
         <v>91</v>
       </c>
@@ -13241,7 +13220,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="170" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:27">
       <c r="A170">
         <v>91</v>
       </c>
@@ -13318,7 +13297,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="171" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:27">
       <c r="A171">
         <v>91</v>
       </c>
@@ -13395,7 +13374,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="172" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:27">
       <c r="A172">
         <v>91</v>
       </c>
@@ -13472,7 +13451,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="173" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:27">
       <c r="A173">
         <v>91</v>
       </c>
@@ -13549,7 +13528,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="174" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:27">
       <c r="A174">
         <v>91</v>
       </c>
@@ -13626,7 +13605,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="175" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:27">
       <c r="A175">
         <v>91</v>
       </c>
@@ -13703,7 +13682,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="176" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:27">
       <c r="A176">
         <v>91</v>
       </c>
@@ -13783,7 +13762,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="177" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:27">
       <c r="A177">
         <v>91</v>
       </c>
@@ -13860,7 +13839,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="178" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:27">
       <c r="A178">
         <v>91</v>
       </c>
@@ -13937,7 +13916,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="179" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:27">
       <c r="A179">
         <v>91</v>
       </c>
@@ -14014,7 +13993,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="180" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:27">
       <c r="A180">
         <v>91</v>
       </c>
@@ -14091,7 +14070,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="181" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:27">
       <c r="A181">
         <v>91</v>
       </c>
@@ -14168,7 +14147,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="182" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:27">
       <c r="A182">
         <v>91</v>
       </c>
@@ -14233,7 +14212,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="183" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:27">
       <c r="A183">
         <v>91</v>
       </c>
@@ -14298,7 +14277,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="184" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:27">
       <c r="A184">
         <v>91</v>
       </c>
@@ -14363,7 +14342,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="185" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:27">
       <c r="A185">
         <v>91</v>
       </c>
@@ -14428,7 +14407,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="186" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:27">
       <c r="A186">
         <v>91</v>
       </c>
@@ -14505,7 +14484,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="187" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:27">
       <c r="A187">
         <v>91</v>
       </c>
@@ -14570,7 +14549,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="188" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:27">
       <c r="A188">
         <v>91</v>
       </c>
@@ -14647,7 +14626,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="189" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:27">
       <c r="A189">
         <v>91</v>
       </c>
@@ -14724,7 +14703,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="190" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:27">
       <c r="A190">
         <v>91</v>
       </c>
@@ -14801,7 +14780,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="191" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:27">
       <c r="A191">
         <v>91</v>
       </c>
@@ -14866,7 +14845,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="192" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:27">
       <c r="A192">
         <v>91</v>
       </c>
@@ -14931,7 +14910,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="193" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:27">
       <c r="A193">
         <v>91</v>
       </c>
@@ -15008,7 +14987,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="194" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:27">
       <c r="A194">
         <v>91</v>
       </c>
@@ -15085,7 +15064,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="195" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:27">
       <c r="A195">
         <v>91</v>
       </c>
@@ -15162,7 +15141,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="196" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:27">
       <c r="A196">
         <v>91</v>
       </c>
@@ -15239,7 +15218,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="197" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:27">
       <c r="A197">
         <v>91</v>
       </c>
@@ -15304,7 +15283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:27">
       <c r="A198">
         <v>91</v>
       </c>
@@ -15369,7 +15348,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="199" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:27">
       <c r="A199">
         <v>91</v>
       </c>
@@ -15446,7 +15425,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="200" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:27">
       <c r="A200">
         <v>91</v>
       </c>
@@ -15523,7 +15502,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="201" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:27">
       <c r="A201">
         <v>91</v>
       </c>
@@ -15603,7 +15582,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="202" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:27">
       <c r="A202">
         <v>91</v>
       </c>
@@ -15680,7 +15659,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="203" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:27">
       <c r="A203">
         <v>91</v>
       </c>
@@ -15757,7 +15736,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="204" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:27">
       <c r="A204">
         <v>91</v>
       </c>
@@ -15834,7 +15813,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="205" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:27">
       <c r="A205">
         <v>91</v>
       </c>
@@ -15914,7 +15893,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="206" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:27">
       <c r="A206">
         <v>91</v>
       </c>
@@ -15991,7 +15970,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="207" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:27">
       <c r="A207">
         <v>91</v>
       </c>
@@ -16071,7 +16050,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="208" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:27">
       <c r="A208">
         <v>91</v>
       </c>
@@ -16148,7 +16127,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="209" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:27">
       <c r="A209">
         <v>91</v>
       </c>
@@ -16213,7 +16192,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="210" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:27">
       <c r="A210">
         <v>91</v>
       </c>
@@ -16278,7 +16257,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="211" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:27">
       <c r="A211">
         <v>91</v>
       </c>
@@ -16355,7 +16334,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="212" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:27">
       <c r="A212">
         <v>91</v>
       </c>
@@ -16432,7 +16411,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="213" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:27">
       <c r="A213">
         <v>91</v>
       </c>
@@ -16509,7 +16488,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="214" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:27">
       <c r="A214">
         <v>91</v>
       </c>
@@ -16586,7 +16565,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="215" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:27">
       <c r="A215">
         <v>91</v>
       </c>
@@ -16666,7 +16645,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="216" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:27">
       <c r="A216">
         <v>91</v>
       </c>
@@ -16746,7 +16725,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="217" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:27">
       <c r="A217">
         <v>91</v>
       </c>
@@ -16826,7 +16805,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="218" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:27">
       <c r="A218">
         <v>91</v>
       </c>
@@ -16909,7 +16888,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="219" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:27">
       <c r="A219">
         <v>91</v>
       </c>
@@ -16986,7 +16965,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="220" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:27">
       <c r="A220">
         <v>91</v>
       </c>
@@ -17069,7 +17048,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="221" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:27">
       <c r="A221">
         <v>91</v>
       </c>
@@ -17149,7 +17128,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="222" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:27">
       <c r="A222">
         <v>91</v>
       </c>
@@ -17229,7 +17208,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="223" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:27">
       <c r="A223">
         <v>91</v>
       </c>
@@ -17309,7 +17288,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="224" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:27">
       <c r="A224">
         <v>91</v>
       </c>
@@ -17386,7 +17365,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="225" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:27">
       <c r="A225">
         <v>91</v>
       </c>
@@ -17463,7 +17442,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="226" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:27">
       <c r="A226">
         <v>91</v>
       </c>
@@ -17528,7 +17507,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="227" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:27">
       <c r="A227">
         <v>91</v>
       </c>
@@ -17605,7 +17584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="228" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:27">
       <c r="A228">
         <v>91</v>
       </c>
@@ -17682,7 +17661,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="229" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:27">
       <c r="A229">
         <v>91</v>
       </c>
@@ -17759,7 +17738,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="230" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:27">
       <c r="A230">
         <v>91</v>
       </c>
@@ -17836,7 +17815,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="231" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:27">
       <c r="A231">
         <v>91</v>
       </c>
@@ -17913,7 +17892,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="232" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:27">
       <c r="A232">
         <v>91</v>
       </c>
@@ -17990,7 +17969,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="233" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:27">
       <c r="A233">
         <v>91</v>
       </c>
@@ -18055,7 +18034,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="234" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:27">
       <c r="A234">
         <v>91</v>
       </c>
@@ -18132,7 +18111,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="235" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:27">
       <c r="A235">
         <v>91</v>
       </c>
@@ -18209,7 +18188,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="236" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:27">
       <c r="A236">
         <v>91</v>
       </c>
@@ -18286,7 +18265,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="237" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:27">
       <c r="A237">
         <v>91</v>
       </c>
@@ -18363,7 +18342,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="238" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:27">
       <c r="A238">
         <v>91</v>
       </c>
@@ -18443,7 +18422,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="239" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:27">
       <c r="A239">
         <v>91</v>
       </c>
@@ -18526,7 +18505,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="240" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:27">
       <c r="A240">
         <v>91</v>
       </c>
@@ -18606,7 +18585,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="241" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:27">
       <c r="A241">
         <v>91</v>
       </c>
@@ -18683,7 +18662,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="242" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:27">
       <c r="A242">
         <v>91</v>
       </c>
@@ -18760,7 +18739,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="243" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:27">
       <c r="A243">
         <v>91</v>
       </c>
@@ -18837,7 +18816,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="244" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:27">
       <c r="A244">
         <v>91</v>
       </c>
@@ -18914,7 +18893,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="245" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:27">
       <c r="A245">
         <v>91</v>
       </c>
@@ -18994,7 +18973,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="246" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:27">
       <c r="A246">
         <v>91</v>
       </c>
@@ -19074,7 +19053,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="247" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:27">
       <c r="A247">
         <v>91</v>
       </c>
@@ -19154,7 +19133,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="248" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:27">
       <c r="A248">
         <v>91</v>
       </c>
@@ -19234,7 +19213,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="249" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:27">
       <c r="A249">
         <v>91</v>
       </c>
@@ -19314,7 +19293,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="250" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:27">
       <c r="A250">
         <v>91</v>
       </c>
@@ -19394,7 +19373,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="251" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:27">
       <c r="A251">
         <v>91</v>
       </c>
@@ -19474,7 +19453,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="252" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:27">
       <c r="A252">
         <v>91</v>
       </c>
@@ -19554,7 +19533,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="253" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:27">
       <c r="A253">
         <v>91</v>
       </c>
@@ -19634,7 +19613,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="254" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:27">
       <c r="A254">
         <v>91</v>
       </c>
@@ -19711,7 +19690,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="255" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:27">
       <c r="A255">
         <v>91</v>
       </c>
@@ -19791,7 +19770,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="256" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:27">
       <c r="A256">
         <v>91</v>
       </c>
@@ -19868,7 +19847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="257" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:27">
       <c r="A257">
         <v>91</v>
       </c>
@@ -19942,7 +19921,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="258" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:27">
       <c r="A258">
         <v>91</v>
       </c>
@@ -20007,7 +19986,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="259" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:27">
       <c r="A259">
         <v>91</v>
       </c>
@@ -20072,7 +20051,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="260" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:27">
       <c r="A260">
         <v>91</v>
       </c>
@@ -20149,7 +20128,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="261" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:27">
       <c r="A261">
         <v>91</v>
       </c>
@@ -20229,7 +20208,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="262" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:27">
       <c r="A262">
         <v>91</v>
       </c>
@@ -20306,7 +20285,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="263" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:27">
       <c r="A263">
         <v>91</v>
       </c>
@@ -20383,7 +20362,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="264" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:27">
       <c r="A264">
         <v>91</v>
       </c>
@@ -20463,7 +20442,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="265" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:27">
       <c r="A265">
         <v>91</v>
       </c>
@@ -20543,7 +20522,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="266" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:27">
       <c r="A266">
         <v>91</v>
       </c>
@@ -20623,7 +20602,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="267" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:27">
       <c r="A267">
         <v>91</v>
       </c>
@@ -20703,7 +20682,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="268" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:27">
       <c r="A268">
         <v>91</v>
       </c>
@@ -20780,7 +20759,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="269" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:27">
       <c r="A269">
         <v>91</v>
       </c>
@@ -20857,7 +20836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="270" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:27">
       <c r="A270">
         <v>91</v>
       </c>
@@ -20934,7 +20913,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="271" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:27">
       <c r="A271">
         <v>91</v>
       </c>
@@ -21014,7 +20993,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="272" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:27">
       <c r="A272">
         <v>91</v>
       </c>
@@ -21091,7 +21070,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="273" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:27">
       <c r="A273">
         <v>91</v>
       </c>
@@ -21168,7 +21147,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="274" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:27">
       <c r="A274">
         <v>91</v>
       </c>
@@ -21233,7 +21212,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="275" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:27">
       <c r="A275">
         <v>91</v>
       </c>
@@ -21310,7 +21289,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="276" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:27">
       <c r="A276">
         <v>91</v>
       </c>
@@ -21390,7 +21369,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="277" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:27">
       <c r="A277">
         <v>91</v>
       </c>
@@ -21473,7 +21452,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="278" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:27">
       <c r="A278">
         <v>91</v>
       </c>
@@ -21550,7 +21529,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="279" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:27">
       <c r="A279">
         <v>91</v>
       </c>
@@ -21615,7 +21594,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="280" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:27">
       <c r="A280">
         <v>91</v>
       </c>
@@ -21692,7 +21671,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="281" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:27">
       <c r="A281">
         <v>91</v>
       </c>
@@ -21772,7 +21751,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="282" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:27">
       <c r="A282">
         <v>91</v>
       </c>
@@ -21852,7 +21831,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="283" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:27">
       <c r="A283">
         <v>91</v>
       </c>
@@ -21917,7 +21896,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="284" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:27">
       <c r="A284">
         <v>91</v>
       </c>
@@ -21997,7 +21976,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="285" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:27">
       <c r="A285">
         <v>91</v>
       </c>
@@ -22074,7 +22053,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="286" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:27">
       <c r="A286">
         <v>91</v>
       </c>
@@ -22154,7 +22133,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="287" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:27">
       <c r="A287">
         <v>91</v>
       </c>
@@ -22231,7 +22210,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="288" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:27">
       <c r="A288">
         <v>91</v>
       </c>
@@ -22296,7 +22275,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="289" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:27">
       <c r="A289">
         <v>91</v>
       </c>
@@ -22373,7 +22352,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:27">
       <c r="A290">
         <v>91</v>
       </c>
@@ -22450,7 +22429,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="291" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:27">
       <c r="A291">
         <v>91</v>
       </c>
@@ -22530,7 +22509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:27">
       <c r="A292">
         <v>91</v>
       </c>
@@ -22610,7 +22589,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="293" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:27">
       <c r="A293">
         <v>91</v>
       </c>
@@ -22687,7 +22666,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="294" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:27">
       <c r="A294">
         <v>91</v>
       </c>
@@ -22767,7 +22746,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="295" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:27">
       <c r="A295">
         <v>91</v>
       </c>
@@ -22847,7 +22826,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="296" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:27">
       <c r="A296">
         <v>91</v>
       </c>
@@ -22930,7 +22909,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="297" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:27">
       <c r="A297">
         <v>91</v>
       </c>
@@ -23013,7 +22992,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="298" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:27">
       <c r="A298">
         <v>91</v>
       </c>
@@ -23093,7 +23072,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="299" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:27">
       <c r="A299">
         <v>91</v>
       </c>
@@ -23158,7 +23137,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="300" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:27">
       <c r="A300">
         <v>91</v>
       </c>
@@ -23223,7 +23202,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="301" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:27">
       <c r="A301">
         <v>91</v>
       </c>
@@ -23300,7 +23279,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="302" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:27">
       <c r="A302">
         <v>91</v>
       </c>
@@ -23377,7 +23356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="303" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:27">
       <c r="A303">
         <v>91</v>
       </c>
@@ -23442,7 +23421,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="304" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:27">
       <c r="A304">
         <v>91</v>
       </c>
@@ -23519,7 +23498,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="305" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:27">
       <c r="A305">
         <v>91</v>
       </c>
@@ -23584,7 +23563,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="306" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:27">
       <c r="A306">
         <v>91</v>
       </c>
@@ -23649,7 +23628,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="307" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:27">
       <c r="A307">
         <v>91</v>
       </c>
@@ -23729,7 +23708,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="308" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:27">
       <c r="A308">
         <v>91</v>
       </c>
@@ -23806,7 +23785,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="309" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:27">
       <c r="A309">
         <v>91</v>
       </c>
@@ -23883,7 +23862,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="310" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:27">
       <c r="A310">
         <v>91</v>
       </c>
@@ -23960,7 +23939,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="311" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:27">
       <c r="A311">
         <v>91</v>
       </c>
@@ -24037,7 +24016,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="312" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:27">
       <c r="A312">
         <v>91</v>
       </c>
@@ -24117,7 +24096,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="313" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:27">
       <c r="A313">
         <v>91</v>
       </c>
@@ -24194,7 +24173,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="314" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:27">
       <c r="A314">
         <v>91</v>
       </c>
@@ -24271,7 +24250,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="315" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:27">
       <c r="A315">
         <v>91</v>
       </c>
@@ -24348,7 +24327,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="316" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:27">
       <c r="A316">
         <v>91</v>
       </c>
@@ -24428,7 +24407,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="317" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:27">
       <c r="A317">
         <v>91</v>
       </c>
@@ -24505,7 +24484,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="318" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:27">
       <c r="A318">
         <v>91</v>
       </c>
@@ -24588,7 +24567,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="319" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:27">
       <c r="A319">
         <v>91</v>
       </c>
@@ -24671,7 +24650,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="320" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:27">
       <c r="A320">
         <v>91</v>
       </c>
@@ -24754,7 +24733,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="321" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:27">
       <c r="A321">
         <v>91</v>
       </c>
@@ -24831,7 +24810,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="322" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:27">
       <c r="A322">
         <v>91</v>
       </c>
@@ -24896,7 +24875,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="323" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:27">
       <c r="A323">
         <v>91</v>
       </c>
@@ -24961,7 +24940,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="324" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:27">
       <c r="A324">
         <v>91</v>
       </c>
@@ -25038,7 +25017,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="325" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:27">
       <c r="A325">
         <v>91</v>
       </c>
@@ -25115,7 +25094,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="326" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:27">
       <c r="A326">
         <v>91</v>
       </c>
@@ -25180,7 +25159,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="327" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:27">
       <c r="A327">
         <v>91</v>
       </c>
@@ -25257,7 +25236,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="328" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:27">
       <c r="A328">
         <v>91</v>
       </c>
@@ -25334,7 +25313,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="329" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:27">
       <c r="A329">
         <v>91</v>
       </c>
@@ -25414,7 +25393,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="330" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:27">
       <c r="A330">
         <v>91</v>
       </c>
@@ -25497,7 +25476,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="331" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:27">
       <c r="A331">
         <v>91</v>
       </c>
@@ -25574,7 +25553,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="332" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:27">
       <c r="A332">
         <v>91</v>
       </c>
@@ -25651,7 +25630,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="333" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:27">
       <c r="A333">
         <v>91</v>
       </c>
@@ -25716,7 +25695,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="334" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:27">
       <c r="A334">
         <v>91</v>
       </c>
@@ -25796,7 +25775,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="335" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:27">
       <c r="A335">
         <v>91</v>
       </c>
@@ -25873,7 +25852,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="336" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:27">
       <c r="A336">
         <v>91</v>
       </c>
@@ -25950,7 +25929,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="337" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:27">
       <c r="A337">
         <v>91</v>
       </c>
@@ -26027,7 +26006,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="338" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:27">
       <c r="A338">
         <v>91</v>
       </c>
@@ -26104,7 +26083,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="339" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:27">
       <c r="A339">
         <v>91</v>
       </c>
@@ -26181,7 +26160,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="340" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:27">
       <c r="A340">
         <v>91</v>
       </c>
@@ -26258,7 +26237,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="341" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:27">
       <c r="A341">
         <v>91</v>
       </c>
@@ -26338,7 +26317,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="342" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:27">
       <c r="A342">
         <v>91</v>
       </c>
@@ -26418,7 +26397,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="343" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:27">
       <c r="A343">
         <v>91</v>
       </c>
@@ -26495,7 +26474,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="344" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:27">
       <c r="A344">
         <v>91</v>
       </c>
@@ -26560,7 +26539,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="345" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:27">
       <c r="A345">
         <v>91</v>
       </c>
@@ -26625,7 +26604,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="346" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:27">
       <c r="A346">
         <v>91</v>
       </c>
@@ -26702,7 +26681,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="347" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:27">
       <c r="A347">
         <v>91</v>
       </c>
@@ -26785,7 +26764,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="348" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:27">
       <c r="A348">
         <v>91</v>
       </c>
@@ -26868,7 +26847,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="349" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:27">
       <c r="A349">
         <v>91</v>
       </c>
@@ -26945,7 +26924,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="350" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:27">
       <c r="A350">
         <v>91</v>
       </c>
@@ -27025,7 +27004,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="351" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:27">
       <c r="A351">
         <v>91</v>
       </c>
@@ -27108,7 +27087,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="352" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:27">
       <c r="A352">
         <v>91</v>
       </c>
@@ -27185,7 +27164,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="353" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:27">
       <c r="A353">
         <v>91</v>
       </c>
@@ -27265,7 +27244,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="354" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:27">
       <c r="A354">
         <v>91</v>
       </c>
@@ -27342,7 +27321,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="355" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:27">
       <c r="A355">
         <v>91</v>
       </c>
@@ -27419,7 +27398,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="356" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:27">
       <c r="A356">
         <v>91</v>
       </c>
@@ -27499,7 +27478,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="357" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:27">
       <c r="A357">
         <v>91</v>
       </c>
@@ -27579,7 +27558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:27">
       <c r="A358">
         <v>91</v>
       </c>
@@ -27659,7 +27638,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="359" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:27">
       <c r="A359">
         <v>91</v>
       </c>
@@ -27736,7 +27715,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="360" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:27">
       <c r="A360">
         <v>91</v>
       </c>
@@ -27813,7 +27792,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="361" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:27">
       <c r="A361">
         <v>91</v>
       </c>
@@ -27878,7 +27857,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="362" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:27">
       <c r="A362">
         <v>91</v>
       </c>
@@ -27943,7 +27922,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="363" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:27">
       <c r="A363">
         <v>91</v>
       </c>
@@ -28023,7 +28002,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="364" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:27">
       <c r="A364">
         <v>91</v>
       </c>
@@ -28103,7 +28082,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="365" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:27">
       <c r="A365">
         <v>91</v>
       </c>
@@ -28180,7 +28159,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="366" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:27">
       <c r="A366">
         <v>91</v>
       </c>
@@ -28256,7 +28235,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28268,7 +28247,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>